<commit_message>
HW3 graphs for 64 core machine
</commit_message>
<xml_diff>
--- a/HW3_Graphs.xlsx
+++ b/HW3_Graphs.xlsx
@@ -212,8 +212,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -276,7 +278,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -290,6 +292,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -303,6 +306,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,11 +436,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125241448"/>
-        <c:axId val="2125248312"/>
+        <c:axId val="2038727352"/>
+        <c:axId val="2065387832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125241448"/>
+        <c:axId val="2038727352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -464,7 +468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125248312"/>
+        <c:crossAx val="2065387832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -472,7 +476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125248312"/>
+        <c:axId val="2065387832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125241448"/>
+        <c:crossAx val="2038727352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -683,11 +687,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125319176"/>
-        <c:axId val="2125324968"/>
+        <c:axId val="2066308888"/>
+        <c:axId val="2066314680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125319176"/>
+        <c:axId val="2066308888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125324968"/>
+        <c:crossAx val="2066314680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -751,7 +755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125324968"/>
+        <c:axId val="2066314680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125319176"/>
+        <c:crossAx val="2066308888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1230,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C42" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>